<commit_message>
Added computations for week-by-week additions of posts.
</commit_message>
<xml_diff>
--- a/stats/cs229/cs229AllIncrementals.xlsx
+++ b/stats/cs229/cs229AllIncrementals.xlsx
@@ -21,7 +21,7 @@
     <sheet name="CS229Fall12" sheetId="8" r:id="rId7"/>
     <sheet name="CS229Fall11" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -126,8 +126,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,11 +145,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,26 +520,26 @@
         <v>4.2396162196618199E-3</v>
       </c>
       <c r="D3">
-        <f>$D2</f>
+        <f t="shared" ref="D3:D14" si="0">$D2</f>
         <v>9.596884128529668</v>
       </c>
       <c r="E3" s="3">
         <v>-16.864654300000002</v>
       </c>
       <c r="F3">
-        <f>F2+B3-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" ref="F3:F14" si="1">F2+B3-AVERAGE($B$2:$B$14)</f>
         <v>-16.864654333008716</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G14" si="0">STDEV($B$2:$B$14)</f>
+        <f t="shared" ref="G3:G14" si="2">STDEV($B$2:$B$14)</f>
         <v>5.8415237961064026</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="1">$C$2+2*$G$2</f>
+        <f t="shared" ref="H3:H14" si="3">$C$2+2*$G$2</f>
         <v>11.688120054158786</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I14" si="2">$D$2-2*$G$2</f>
+        <f t="shared" ref="I3:I14" si="4">$D$2-2*$G$2</f>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -546,26 +554,26 @@
         <v>5.0428368731815299E-3</v>
       </c>
       <c r="D4">
-        <f>$D3</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E4" s="3">
         <v>-23.4741967</v>
       </c>
       <c r="F4">
-        <f>F3+B4-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-23.474196689386496</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -580,26 +588,26 @@
         <v>4.9406893969737697E-3</v>
       </c>
       <c r="D5">
-        <f>$D4</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E5" s="3">
         <v>-27.590068200000001</v>
       </c>
       <c r="F5">
-        <f>F4+B5-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-27.590068159688322</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -614,26 +622,26 @@
         <v>5.2986154306750603E-3</v>
       </c>
       <c r="D6">
-        <f>$D5</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E6" s="3">
         <v>-30.705939600000001</v>
       </c>
       <c r="F6">
-        <f>F5+B6-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-30.705939629990148</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -648,26 +656,26 @@
         <v>5.2445084517638097E-3</v>
       </c>
       <c r="D7">
-        <f>$D6</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E7" s="3">
         <v>-32.366114899999999</v>
       </c>
       <c r="F7">
-        <f>F6+B7-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-32.366114897760326</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -682,26 +690,26 @@
         <v>5.4344298784223203E-3</v>
       </c>
       <c r="D8">
-        <f>$D7</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E8" s="3">
         <v>-32.899707900000003</v>
       </c>
       <c r="F8">
-        <f>F7+B8-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-32.899707887049495</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -716,26 +724,26 @@
         <v>6.1663472563660403E-3</v>
       </c>
       <c r="D9">
-        <f>$D8</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E9" s="3">
         <v>-29.9269718</v>
       </c>
       <c r="F9">
-        <f>F8+B9-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-29.926971762414659</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -750,26 +758,26 @@
         <v>6.3706285150564798E-3</v>
       </c>
       <c r="D10">
-        <f>$D9</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E10" s="3">
         <v>-25.777020400000001</v>
       </c>
       <c r="F10">
-        <f>F9+B10-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-25.777020447906423</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -784,26 +792,26 @@
         <v>6.6226898907881301E-3</v>
       </c>
       <c r="D11">
-        <f>$D10</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E11" s="3">
         <v>-20.310613400000001</v>
       </c>
       <c r="F11">
-        <f>F10+B11-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-20.310613437195592</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -818,26 +826,26 @@
         <v>6.9553366875417001E-3</v>
       </c>
       <c r="D12">
-        <f>$D11</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E12" s="3">
         <v>-13.9201558</v>
       </c>
       <c r="F12">
-        <f>F11+B12-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-13.920155793573461</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -852,26 +860,26 @@
         <v>7.3369027841488996E-3</v>
       </c>
       <c r="D13">
-        <f>$D12</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E13" s="3">
         <v>-7.0486854900000004</v>
       </c>
       <c r="F13">
-        <f>F12+B13-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>-7.0486854917234272</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -886,26 +894,26 @@
         <v>7.3332460225109999E-3</v>
       </c>
       <c r="D14">
-        <f>$D13</f>
+        <f t="shared" si="0"/>
         <v>9.596884128529668</v>
       </c>
       <c r="E14" s="3">
         <v>5.3290705200000003E-15</v>
       </c>
       <c r="F14">
-        <f>F13+B14-AVERAGE($B$2:$B$14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8415237961064026</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.688120054158786</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.0861634636831372</v>
       </c>
     </row>
@@ -1009,7 +1017,7 @@
         <v>49.643374678756729</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="F3:G11" si="3">$C$2-2*$E$2</f>
+        <f t="shared" ref="G3:G11" si="3">$C$2-2*$E$2</f>
         <v>-5.030041345423431</v>
       </c>
     </row>
@@ -1259,7 +1267,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C15"/>
+      <selection activeCell="A3" sqref="A3:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1308,7 @@
         <v>1.62025316455696</v>
       </c>
       <c r="C3">
-        <f>B3-C2</f>
+        <f t="shared" ref="C3:C12" si="0">B3-C2</f>
         <v>1.62025316455696</v>
       </c>
     </row>
@@ -1312,7 +1320,7 @@
         <v>2.43037974683544</v>
       </c>
       <c r="C4">
-        <f>B4-C3</f>
+        <f t="shared" si="0"/>
         <v>0.81012658227848</v>
       </c>
     </row>
@@ -1324,7 +1332,7 @@
         <v>4.9113924050632898</v>
       </c>
       <c r="C5">
-        <f>B5-C4</f>
+        <f t="shared" si="0"/>
         <v>4.1012658227848098</v>
       </c>
     </row>
@@ -1336,7 +1344,7 @@
         <v>7.5949367088607502</v>
       </c>
       <c r="C6">
-        <f>B6-C5</f>
+        <f t="shared" si="0"/>
         <v>3.4936708860759405</v>
       </c>
     </row>
@@ -1348,7 +1356,7 @@
         <v>9.6962025316455698</v>
       </c>
       <c r="C7">
-        <f>B7-C6</f>
+        <f t="shared" si="0"/>
         <v>6.2025316455696293</v>
       </c>
     </row>
@@ -1360,7 +1368,7 @@
         <v>11.9240506329113</v>
       </c>
       <c r="C8">
-        <f>B8-C7</f>
+        <f t="shared" si="0"/>
         <v>5.7215189873416703</v>
       </c>
     </row>
@@ -1372,7 +1380,7 @@
         <v>13.6708860759493</v>
       </c>
       <c r="C9">
-        <f>B9-C8</f>
+        <f t="shared" si="0"/>
         <v>7.9493670886076293</v>
       </c>
     </row>
@@ -1384,7 +1392,7 @@
         <v>17.683544303797401</v>
       </c>
       <c r="C10">
-        <f>B10-C9</f>
+        <f t="shared" si="0"/>
         <v>9.7341772151897707</v>
       </c>
     </row>
@@ -1396,7 +1404,7 @@
         <v>19.329113924050599</v>
       </c>
       <c r="C11">
-        <f>B11-C10</f>
+        <f t="shared" si="0"/>
         <v>9.5949367088608284</v>
       </c>
     </row>
@@ -1408,7 +1416,7 @@
         <v>21.164556962025301</v>
       </c>
       <c r="C12">
-        <f>B12-C11</f>
+        <f t="shared" si="0"/>
         <v>11.569620253164473</v>
       </c>
     </row>
@@ -1420,7 +1428,7 @@
         <v>23.050632911392398</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C15" si="0">B13-C12</f>
+        <f t="shared" ref="C13:C15" si="1">B13-C12</f>
         <v>11.481012658227925</v>
       </c>
     </row>
@@ -1432,7 +1440,7 @@
         <v>23.772151898734101</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.291139240506176</v>
       </c>
     </row>
@@ -1444,7 +1452,7 @@
         <v>24.025316455696199</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.734177215190023</v>
       </c>
     </row>
@@ -1459,7 +1467,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1647,7 +1655,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C3" sqref="C3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1842,7 +1850,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C3" sqref="C3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1874,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <f>B3-C2</f>
+        <f t="shared" ref="C3:C12" si="0">B3-C2</f>
         <v>3</v>
       </c>
     </row>
@@ -1886,7 +1894,7 @@
         <v>4.5584415584415501</v>
       </c>
       <c r="C4">
-        <f>B4-C3</f>
+        <f t="shared" si="0"/>
         <v>1.5584415584415501</v>
       </c>
     </row>
@@ -1898,7 +1906,7 @@
         <v>7.62337662337662</v>
       </c>
       <c r="C5">
-        <f>B5-C4</f>
+        <f t="shared" si="0"/>
         <v>6.06493506493507</v>
       </c>
     </row>
@@ -1910,7 +1918,7 @@
         <v>10.363636363636299</v>
       </c>
       <c r="C6">
-        <f>B6-C5</f>
+        <f t="shared" si="0"/>
         <v>4.2987012987012294</v>
       </c>
     </row>
@@ -1922,7 +1930,7 @@
         <v>14.545454545454501</v>
       </c>
       <c r="C7">
-        <f>B7-C6</f>
+        <f t="shared" si="0"/>
         <v>10.246753246753272</v>
       </c>
     </row>
@@ -1934,7 +1942,7 @@
         <v>17.025974025974001</v>
       </c>
       <c r="C8">
-        <f>B8-C7</f>
+        <f t="shared" si="0"/>
         <v>6.7792207792207293</v>
       </c>
     </row>
@@ -1946,7 +1954,7 @@
         <v>20.402597402597401</v>
       </c>
       <c r="C9">
-        <f>B9-C8</f>
+        <f t="shared" si="0"/>
         <v>13.623376623376672</v>
       </c>
     </row>
@@ -1958,7 +1966,7 @@
         <v>22.506493506493499</v>
       </c>
       <c r="C10">
-        <f>B10-C9</f>
+        <f t="shared" si="0"/>
         <v>8.883116883116827</v>
       </c>
     </row>
@@ -1970,7 +1978,7 @@
         <v>24.6753246753246</v>
       </c>
       <c r="C11">
-        <f>B11-C10</f>
+        <f t="shared" si="0"/>
         <v>15.792207792207773</v>
       </c>
     </row>
@@ -1982,7 +1990,7 @@
         <v>26.4545454545454</v>
       </c>
       <c r="C12">
-        <f>B12-C11</f>
+        <f t="shared" si="0"/>
         <v>10.662337662337627</v>
       </c>
     </row>
@@ -1994,7 +2002,7 @@
         <v>28.792207792207702</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C15" si="0">B13-C12</f>
+        <f t="shared" ref="C13:C15" si="1">B13-C12</f>
         <v>18.129870129870074</v>
       </c>
     </row>
@@ -2006,7 +2014,7 @@
         <v>29.350649350649299</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.220779220779225</v>
       </c>
     </row>
@@ -2018,7 +2026,7 @@
         <v>29.3766233766233</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.155844155844076</v>
       </c>
     </row>
@@ -2032,7 +2040,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C3" sqref="C3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2064,7 +2072,7 @@
         <v>1.8793103448275801</v>
       </c>
       <c r="C3">
-        <f>B3-C2</f>
+        <f t="shared" ref="C3:C12" si="0">B3-C2</f>
         <v>1.8793103448275801</v>
       </c>
     </row>
@@ -2076,7 +2084,7 @@
         <v>3.5</v>
       </c>
       <c r="C4">
-        <f>B4-C3</f>
+        <f t="shared" si="0"/>
         <v>1.6206896551724199</v>
       </c>
     </row>
@@ -2088,7 +2096,7 @@
         <v>5.7413793103448203</v>
       </c>
       <c r="C5">
-        <f>B5-C4</f>
+        <f t="shared" si="0"/>
         <v>4.1206896551724004</v>
       </c>
     </row>
@@ -2100,7 +2108,7 @@
         <v>7.63793103448275</v>
       </c>
       <c r="C6">
-        <f>B6-C5</f>
+        <f t="shared" si="0"/>
         <v>3.5172413793103496</v>
       </c>
     </row>
@@ -2112,7 +2120,7 @@
         <v>10.9482758620689</v>
       </c>
       <c r="C7">
-        <f>B7-C6</f>
+        <f t="shared" si="0"/>
         <v>7.4310344827585508</v>
       </c>
     </row>
@@ -2124,7 +2132,7 @@
         <v>13.4482758620689</v>
       </c>
       <c r="C8">
-        <f>B8-C7</f>
+        <f t="shared" si="0"/>
         <v>6.0172413793103496</v>
       </c>
     </row>
@@ -2136,7 +2144,7 @@
         <v>15.189655172413699</v>
       </c>
       <c r="C9">
-        <f>B9-C8</f>
+        <f t="shared" si="0"/>
         <v>9.1724137931033489</v>
       </c>
     </row>
@@ -2148,7 +2156,7 @@
         <v>16.2068965517241</v>
       </c>
       <c r="C10">
-        <f>B10-C9</f>
+        <f t="shared" si="0"/>
         <v>7.0344827586207508</v>
       </c>
     </row>
@@ -2160,7 +2168,7 @@
         <v>17.120689655172399</v>
       </c>
       <c r="C11">
-        <f>B11-C10</f>
+        <f t="shared" si="0"/>
         <v>10.086206896551648</v>
       </c>
     </row>
@@ -2172,7 +2180,7 @@
         <v>19</v>
       </c>
       <c r="C12">
-        <f>B12-C11</f>
+        <f t="shared" si="0"/>
         <v>8.9137931034483522</v>
       </c>
     </row>
@@ -2184,7 +2192,7 @@
         <v>20.120689655172399</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C15" si="0">B13-C12</f>
+        <f t="shared" ref="C13:C15" si="1">B13-C12</f>
         <v>11.206896551724046</v>
       </c>
     </row>
@@ -2196,7 +2204,7 @@
         <v>21.103448275862</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.8965517241379537</v>
       </c>
     </row>
@@ -2208,7 +2216,7 @@
         <v>24.025316455696199</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.128764731558245</v>
       </c>
     </row>
@@ -2222,7 +2230,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C21"/>
+      <selection activeCell="C3" sqref="C3:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2254,7 +2262,7 @@
         <v>0.51428571428571401</v>
       </c>
       <c r="C3">
-        <f>B3-C2</f>
+        <f t="shared" ref="C3:C12" si="0">B3-C2</f>
         <v>0.51428571428571401</v>
       </c>
     </row>
@@ -2266,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>B4-C3</f>
+        <f t="shared" si="0"/>
         <v>0.48571428571428599</v>
       </c>
     </row>
@@ -2278,7 +2286,7 @@
         <v>1.02857142857142</v>
       </c>
       <c r="C5">
-        <f>B5-C4</f>
+        <f t="shared" si="0"/>
         <v>0.54285714285713405</v>
       </c>
     </row>
@@ -2290,7 +2298,7 @@
         <v>1.02857142857142</v>
       </c>
       <c r="C6">
-        <f>B6-C5</f>
+        <f t="shared" si="0"/>
         <v>0.48571428571428599</v>
       </c>
     </row>
@@ -2302,7 +2310,7 @@
         <v>1.51428571428571</v>
       </c>
       <c r="C7">
-        <f>B7-C6</f>
+        <f t="shared" si="0"/>
         <v>1.028571428571424</v>
       </c>
     </row>
@@ -2314,7 +2322,7 @@
         <v>3.02857142857142</v>
       </c>
       <c r="C8">
-        <f>B8-C7</f>
+        <f t="shared" si="0"/>
         <v>1.999999999999996</v>
       </c>
     </row>
@@ -2326,7 +2334,7 @@
         <v>3.3428571428571399</v>
       </c>
       <c r="C9">
-        <f>B9-C8</f>
+        <f t="shared" si="0"/>
         <v>1.3428571428571439</v>
       </c>
     </row>
@@ -2338,7 +2346,7 @@
         <v>3.4285714285714199</v>
       </c>
       <c r="C10">
-        <f>B10-C9</f>
+        <f t="shared" si="0"/>
         <v>2.0857142857142761</v>
       </c>
     </row>
@@ -2350,7 +2358,7 @@
         <v>3.6857142857142802</v>
       </c>
       <c r="C11">
-        <f>B11-C10</f>
+        <f t="shared" si="0"/>
         <v>1.6000000000000041</v>
       </c>
     </row>
@@ -2362,7 +2370,7 @@
         <v>3.77142857142857</v>
       </c>
       <c r="C12">
-        <f>B12-C11</f>
+        <f t="shared" si="0"/>
         <v>2.1714285714285659</v>
       </c>
     </row>
@@ -2374,7 +2382,7 @@
         <v>4.3428571428571399</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C21" si="0">B13-C12</f>
+        <f t="shared" ref="C13:C21" si="1">B13-C12</f>
         <v>2.1714285714285739</v>
       </c>
     </row>
@@ -2386,7 +2394,7 @@
         <v>6.4285714285714199</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.2571428571428456</v>
       </c>
     </row>
@@ -2398,7 +2406,7 @@
         <v>6.71428571428571</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4571428571428644</v>
       </c>
     </row>
@@ -2410,7 +2418,7 @@
         <v>7.0285714285714196</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5714285714285552</v>
       </c>
     </row>
@@ -2422,7 +2430,7 @@
         <v>8.6857142857142797</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1142857142857245</v>
       </c>
     </row>
@@ -2434,7 +2442,7 @@
         <v>8.9714285714285698</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8571428571428452</v>
       </c>
     </row>
@@ -2446,7 +2454,7 @@
         <v>8.9714285714285698</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1142857142857245</v>
       </c>
     </row>
@@ -2458,7 +2466,7 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8857142857142755</v>
       </c>
     </row>
@@ -2470,7 +2478,7 @@
         <v>9.2285714285714207</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3428571428571452</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Several new images of Taylor-software changepoint computations. Addions to .bib file and the main text.
</commit_message>
<xml_diff>
--- a/stats/cs229/cs229AllIncrementals.xlsx
+++ b/stats/cs229/cs229AllIncrementals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14740" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14740" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="cs229_top10_students_with_cusum" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Week</t>
   </si>
@@ -70,6 +70,45 @@
   </si>
   <si>
     <t>WeighteOutIncremental</t>
+  </si>
+  <si>
+    <t>Mean data:</t>
+  </si>
+  <si>
+    <t>Mean diffs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper control limit: </t>
+  </si>
+  <si>
+    <t>Lower control limit:</t>
+  </si>
+  <si>
+    <t>SD data:</t>
+  </si>
+  <si>
+    <t>3SD UCL</t>
+  </si>
+  <si>
+    <t>2SD UCL</t>
+  </si>
+  <si>
+    <t>1SD UCL</t>
+  </si>
+  <si>
+    <t>0.5SD UCL</t>
+  </si>
+  <si>
+    <t>3SD LCL</t>
+  </si>
+  <si>
+    <t>2SD LCL</t>
+  </si>
+  <si>
+    <t>1SD LCL</t>
+  </si>
+  <si>
+    <t>0.5SD LCL</t>
   </si>
 </sst>
 </file>
@@ -1652,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1663,9 +1702,10 @@
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1676,7 +1716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1684,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1695,8 +1735,22 @@
         <f>B3-C2</f>
         <v>0.56790123456790098</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE(B3:B15)</f>
+        <v>10.037037037037008</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <f>F3+0.5*F4/1.128</f>
+        <v>12.392263239780933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1707,8 +1761,22 @@
         <f t="shared" ref="C4:C15" si="0">B4-C3</f>
         <v>0.90123456790122891</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <f>AVERAGE(C3:C15)</f>
+        <v>5.3133903133902942</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <f>F3-3*F4/1.128</f>
+        <v>-4.0943201794265427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1720,7 +1788,7 @@
         <v>1.7530864197530911</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1731,8 +1799,15 @@
         <f t="shared" si="0"/>
         <v>2.8765432098765387</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <f>STDEV(B3:B15)</f>
+        <v>6.1502549813746867</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1743,8 +1818,15 @@
         <f t="shared" si="0"/>
         <v>3.8024691358024714</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7">
+        <f>$F$3+3*$F$6</f>
+        <v>28.48780198116107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1755,8 +1837,15 @@
         <f t="shared" si="0"/>
         <v>5.6913580246913487</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <f>$F$3+2*$F$6</f>
+        <v>22.337546999786383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1767,8 +1856,15 @@
         <f t="shared" si="0"/>
         <v>5.9753086419752517</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9">
+        <f>$F$3+1*$F$6</f>
+        <v>16.187292018411696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1779,8 +1875,15 @@
         <f t="shared" si="0"/>
         <v>7.3950617283950475</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <f>$F$3+0.5*$F$6</f>
+        <v>13.112164527724351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1792,7 +1895,7 @@
         <v>6.9506172839505531</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1803,8 +1906,15 @@
         <f t="shared" si="0"/>
         <v>8.6172839506173471</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12">
+        <f>$F$3-3*$F$6</f>
+        <v>-8.4137279070870523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1815,8 +1925,15 @@
         <f t="shared" si="0"/>
         <v>7.6543209876542537</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13">
+        <f>$F$3-2*$F$6</f>
+        <v>-2.2634729257123656</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1827,8 +1944,15 @@
         <f t="shared" si="0"/>
         <v>9.2222222222222445</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14">
+        <f>$F$3-1*$F$6</f>
+        <v>3.8867820556623212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1838,6 +1962,13 @@
       <c r="C15">
         <f t="shared" si="0"/>
         <v>7.6666666666665559</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15">
+        <f>$F$3-0.5*$F$6</f>
+        <v>6.9619095463496645</v>
       </c>
     </row>
   </sheetData>
@@ -2229,7 +2360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes in response to reviewer feedback
</commit_message>
<xml_diff>
--- a/stats/cs229/cs229AllIncrementals.xlsx
+++ b/stats/cs229/cs229AllIncrementals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1380" windowWidth="24960" windowHeight="14740" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="6160" yWindow="9380" windowWidth="24960" windowHeight="14740" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="cs229_top10_students_with_cusum" sheetId="1" r:id="rId1"/>
@@ -2160,6 +2160,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:val>
             <c:numRef>
               <c:f>CS229Fall15!$B$3:$B$14</c:f>

</xml_diff>